<commit_message>
Selesai koreksi paket 1
</commit_message>
<xml_diff>
--- a/Skor.xlsx
+++ b/Skor.xlsx
@@ -445,7 +445,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,18 +507,33 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
       <c r="N2">
         <f>SUM(B2:M2)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
       <c r="N3">
         <f t="shared" ref="N3:N12" si="0">SUM(B3:M3)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -561,18 +576,27 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gian paket 1 done
</commit_message>
<xml_diff>
--- a/Skor.xlsx
+++ b/Skor.xlsx
@@ -445,7 +445,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +508,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -518,7 +518,7 @@
       </c>
       <c r="N2">
         <f>SUM(B2:M2)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -540,9 +540,12 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Paket 3 selesai dikoreksi
</commit_message>
<xml_diff>
--- a/Skor.xlsx
+++ b/Skor.xlsx
@@ -445,7 +445,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,6 +516,9 @@
       <c r="D2">
         <v>7</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="N2">
         <f>SUM(B2:M2)</f>
         <v>18</v>
@@ -531,9 +534,15 @@
       <c r="C3">
         <v>7</v>
       </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
       <c r="N3">
         <f t="shared" ref="N3:N12" si="0">SUM(B3:M3)</f>
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -543,9 +552,18 @@
       <c r="B4">
         <v>4</v>
       </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -570,9 +588,15 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -582,9 +606,12 @@
       <c r="C8">
         <v>7</v>
       </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -597,9 +624,12 @@
       <c r="C9">
         <v>6</v>
       </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>